<commit_message>
Find the best Parameter
</commit_message>
<xml_diff>
--- a/Marker_list_BU.xlsx
+++ b/Marker_list_BU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiesun/Storage/Work/Projects/Microglial_annotation/Microglial-annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7EB98F-5710-314D-BC2C-2432C66BE69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B1D209-D07E-9E4D-80B4-97FD018BC757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="760" windowWidth="27400" windowHeight="17560" xr2:uid="{154C570F-0952-714B-9412-696B912925D9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="306">
   <si>
     <t>ATM</t>
   </si>
@@ -949,6 +949,9 @@
   </si>
   <si>
     <t>Cell_Cycle: cell cycle</t>
+  </si>
+  <si>
+    <t>SAM: Senescence-associated microglia</t>
   </si>
 </sst>
 </file>
@@ -1532,7 +1535,7 @@
   <dimension ref="A1:K202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1814,7 +1817,9 @@
       <c r="E11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="7"/>
+      <c r="J11" s="7" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">

</xml_diff>